<commit_message>
updated README; added columns to timeline data
</commit_message>
<xml_diff>
--- a/data/method-year.xlsx
+++ b/data/method-year.xlsx
@@ -20,21 +20,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t xml:space="preserve">year</t>
   </si>
   <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
     <t xml:space="preserve">method name</t>
   </si>
   <si>
     <t xml:space="preserve">citation</t>
   </si>
   <si>
+    <t xml:space="preserve">multiple_instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple_outcomes</t>
+  </si>
+  <si>
     <t xml:space="preserve">omnigenic Mendelian randomization</t>
   </si>
   <si>
     <t xml:space="preserve">wang_mendelian_nodate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moPMR-Egger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liu_multi-trait_2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMR-Egger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yuan_testing_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
 </sst>
 </file>
@@ -49,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,16 +158,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -152,13 +182,59 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>